<commit_message>
Fixed test_batch_output_excel octave bug
</commit_message>
<xml_diff>
--- a/test_templates/test_batch_template4.xlsx
+++ b/test_templates/test_batch_template4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-50385" yWindow="1080" windowWidth="47745" windowHeight="25665" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-50385" yWindow="1080" windowWidth="47745" windowHeight="25665" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment" sheetId="6" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="534">
   <si>
     <t>blank plasmid</t>
   </si>
@@ -2617,6 +2617,9 @@
   </si>
   <si>
     <t>Min Valid a.u.</t>
+  </si>
+  <si>
+    <t>10^4</t>
   </si>
 </sst>
 </file>
@@ -4321,41 +4324,113 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4399,59 +4474,26 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4528,13 +4570,10 @@
     <xf numFmtId="0" fontId="15" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4564,6 +4603,15 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4588,45 +4636,6 @@
     <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4660,6 +4669,45 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="18" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4714,51 +4762,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5682,86 +5685,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="257" t="s">
+      <c r="A1" s="279" t="s">
         <v>351</v>
       </c>
-      <c r="B1" s="258"/>
-      <c r="C1" s="258"/>
-      <c r="D1" s="258"/>
-      <c r="E1" s="258"/>
-      <c r="F1" s="258"/>
-      <c r="G1" s="258"/>
-      <c r="H1" s="258"/>
-      <c r="I1" s="258"/>
-      <c r="J1" s="258"/>
-      <c r="K1" s="259"/>
+      <c r="B1" s="280"/>
+      <c r="C1" s="280"/>
+      <c r="D1" s="280"/>
+      <c r="E1" s="280"/>
+      <c r="F1" s="280"/>
+      <c r="G1" s="280"/>
+      <c r="H1" s="280"/>
+      <c r="I1" s="280"/>
+      <c r="J1" s="280"/>
+      <c r="K1" s="281"/>
     </row>
     <row r="2" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="85"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="273" t="s">
+      <c r="A3" s="258" t="s">
         <v>289</v>
       </c>
-      <c r="B3" s="274"/>
+      <c r="B3" s="259"/>
     </row>
     <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="271" t="s">
+      <c r="A4" s="272" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="272"/>
+      <c r="B4" s="273"/>
     </row>
     <row r="5" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="287" t="s">
+      <c r="A5" s="274" t="s">
         <v>182</v>
       </c>
-      <c r="B5" s="288"/>
+      <c r="B5" s="275"/>
     </row>
     <row r="6" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="85"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="273" t="s">
+      <c r="A7" s="258" t="s">
         <v>246</v>
       </c>
-      <c r="B7" s="275"/>
-      <c r="C7" s="275"/>
-      <c r="D7" s="275"/>
-      <c r="E7" s="275"/>
-      <c r="F7" s="275"/>
-      <c r="G7" s="275"/>
-      <c r="H7" s="275"/>
-      <c r="I7" s="275"/>
-      <c r="J7" s="275"/>
-      <c r="K7" s="274"/>
+      <c r="B7" s="260"/>
+      <c r="C7" s="260"/>
+      <c r="D7" s="260"/>
+      <c r="E7" s="260"/>
+      <c r="F7" s="260"/>
+      <c r="G7" s="260"/>
+      <c r="H7" s="260"/>
+      <c r="I7" s="260"/>
+      <c r="J7" s="260"/>
+      <c r="K7" s="259"/>
     </row>
     <row r="8" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="260" t="s">
+      <c r="A8" s="282" t="s">
         <v>162</v>
       </c>
-      <c r="B8" s="261"/>
-      <c r="C8" s="261"/>
-      <c r="D8" s="261"/>
-      <c r="E8" s="261"/>
-      <c r="F8" s="261"/>
-      <c r="G8" s="261"/>
-      <c r="H8" s="261"/>
-      <c r="I8" s="261"/>
-      <c r="J8" s="261"/>
-      <c r="K8" s="262"/>
+      <c r="B8" s="283"/>
+      <c r="C8" s="283"/>
+      <c r="D8" s="283"/>
+      <c r="E8" s="283"/>
+      <c r="F8" s="283"/>
+      <c r="G8" s="283"/>
+      <c r="H8" s="283"/>
+      <c r="I8" s="283"/>
+      <c r="J8" s="283"/>
+      <c r="K8" s="284"/>
     </row>
     <row r="9" spans="1:11" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="263"/>
-      <c r="B9" s="264"/>
-      <c r="C9" s="264"/>
-      <c r="D9" s="264"/>
-      <c r="E9" s="264"/>
-      <c r="F9" s="264"/>
-      <c r="G9" s="264"/>
-      <c r="H9" s="264"/>
-      <c r="I9" s="264"/>
-      <c r="J9" s="264"/>
-      <c r="K9" s="265"/>
+      <c r="A9" s="285"/>
+      <c r="B9" s="286"/>
+      <c r="C9" s="286"/>
+      <c r="D9" s="286"/>
+      <c r="E9" s="286"/>
+      <c r="F9" s="286"/>
+      <c r="G9" s="286"/>
+      <c r="H9" s="286"/>
+      <c r="I9" s="286"/>
+      <c r="J9" s="286"/>
+      <c r="K9" s="287"/>
     </row>
     <row r="10" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="154"/>
@@ -5772,62 +5775,62 @@
       <c r="F10" s="140"/>
     </row>
     <row r="11" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="276" t="s">
+      <c r="A11" s="261" t="s">
         <v>247</v>
       </c>
-      <c r="B11" s="277"/>
-      <c r="C11" s="277"/>
-      <c r="D11" s="278"/>
+      <c r="B11" s="262"/>
+      <c r="C11" s="262"/>
+      <c r="D11" s="263"/>
       <c r="E11" s="86"/>
       <c r="F11" s="140"/>
     </row>
     <row r="12" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="279" t="s">
+      <c r="A12" s="264" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="280"/>
-      <c r="C12" s="281" t="s">
+      <c r="B12" s="265"/>
+      <c r="C12" s="266" t="s">
         <v>164</v>
       </c>
-      <c r="D12" s="282"/>
+      <c r="D12" s="267"/>
       <c r="E12" s="86"/>
       <c r="F12" s="140"/>
     </row>
     <row r="13" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="283"/>
-      <c r="B13" s="284"/>
-      <c r="C13" s="285"/>
-      <c r="D13" s="286"/>
+      <c r="A13" s="268"/>
+      <c r="B13" s="269"/>
+      <c r="C13" s="270"/>
+      <c r="D13" s="271"/>
       <c r="E13" s="86"/>
       <c r="F13" s="140"/>
     </row>
     <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:11" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="276" t="s">
+      <c r="A15" s="261" t="s">
         <v>248</v>
       </c>
-      <c r="B15" s="278"/>
-      <c r="E15" s="276" t="s">
+      <c r="B15" s="263"/>
+      <c r="E15" s="261" t="s">
         <v>288</v>
       </c>
-      <c r="F15" s="277"/>
-      <c r="G15" s="277"/>
-      <c r="H15" s="277"/>
-      <c r="I15" s="278"/>
+      <c r="F15" s="262"/>
+      <c r="G15" s="262"/>
+      <c r="H15" s="262"/>
+      <c r="I15" s="263"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="271" t="s">
+      <c r="A16" s="272" t="s">
         <v>209</v>
       </c>
-      <c r="B16" s="272"/>
+      <c r="B16" s="273"/>
       <c r="D16" s="87"/>
-      <c r="E16" s="266" t="s">
+      <c r="E16" s="288" t="s">
         <v>184</v>
       </c>
-      <c r="F16" s="267"/>
-      <c r="G16" s="267"/>
-      <c r="H16" s="267"/>
-      <c r="I16" s="268"/>
+      <c r="F16" s="289"/>
+      <c r="G16" s="289"/>
+      <c r="H16" s="289"/>
+      <c r="I16" s="290"/>
     </row>
     <row r="17" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="155" t="s">
@@ -5837,10 +5840,10 @@
         <v>251</v>
       </c>
       <c r="C17" s="88"/>
-      <c r="E17" s="269" t="s">
+      <c r="E17" s="291" t="s">
         <v>208</v>
       </c>
-      <c r="F17" s="270"/>
+      <c r="F17" s="292"/>
       <c r="G17" s="192" t="s">
         <v>159</v>
       </c>
@@ -5870,7 +5873,7 @@
       <c r="H18" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="I18" s="245" t="s">
+      <c r="I18" s="276" t="s">
         <v>444</v>
       </c>
       <c r="J18" s="80"/>
@@ -5893,7 +5896,7 @@
       <c r="H19" s="73" t="s">
         <v>183</v>
       </c>
-      <c r="I19" s="245"/>
+      <c r="I19" s="276"/>
       <c r="J19" s="80"/>
     </row>
     <row r="20" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5910,7 +5913,7 @@
       </c>
       <c r="G20" s="70"/>
       <c r="H20" s="70"/>
-      <c r="I20" s="246"/>
+      <c r="I20" s="277"/>
       <c r="J20" s="80"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -5932,24 +5935,24 @@
       <c r="A23" s="159"/>
       <c r="B23" s="91"/>
       <c r="C23" s="90"/>
-      <c r="E23" s="247" t="s">
+      <c r="E23" s="256" t="s">
         <v>185</v>
       </c>
-      <c r="F23" s="248"/>
-      <c r="G23" s="248"/>
-      <c r="H23" s="248"/>
-      <c r="I23" s="249"/>
+      <c r="F23" s="278"/>
+      <c r="G23" s="278"/>
+      <c r="H23" s="278"/>
+      <c r="I23" s="257"/>
     </row>
     <row r="24" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="247" t="s">
+      <c r="A24" s="256" t="s">
         <v>213</v>
       </c>
-      <c r="B24" s="249"/>
+      <c r="B24" s="257"/>
       <c r="C24" s="31"/>
-      <c r="E24" s="253" t="s">
+      <c r="E24" s="296" t="s">
         <v>208</v>
       </c>
-      <c r="F24" s="254"/>
+      <c r="F24" s="297"/>
       <c r="G24" s="192" t="s">
         <v>159</v>
       </c>
@@ -5978,7 +5981,7 @@
       <c r="H25" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="I25" s="250" t="s">
+      <c r="I25" s="293" t="s">
         <v>445</v>
       </c>
     </row>
@@ -6002,7 +6005,7 @@
       <c r="H26" s="73" t="s">
         <v>188</v>
       </c>
-      <c r="I26" s="251"/>
+      <c r="I26" s="294"/>
     </row>
     <row r="27" spans="1:10" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="157" t="s">
@@ -6018,7 +6021,7 @@
       </c>
       <c r="G27" s="70"/>
       <c r="H27" s="70"/>
-      <c r="I27" s="252"/>
+      <c r="I27" s="295"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="157" t="s">
@@ -6042,22 +6045,22 @@
       <c r="A30" s="158"/>
       <c r="B30" s="115"/>
       <c r="C30" s="88"/>
-      <c r="E30" s="247" t="s">
+      <c r="E30" s="256" t="s">
         <v>186</v>
       </c>
-      <c r="F30" s="248"/>
-      <c r="G30" s="248"/>
-      <c r="H30" s="248"/>
-      <c r="I30" s="249"/>
+      <c r="F30" s="278"/>
+      <c r="G30" s="278"/>
+      <c r="H30" s="278"/>
+      <c r="I30" s="257"/>
     </row>
     <row r="31" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="159"/>
       <c r="B31" s="90"/>
       <c r="C31" s="90"/>
-      <c r="E31" s="255" t="s">
+      <c r="E31" s="298" t="s">
         <v>430</v>
       </c>
-      <c r="F31" s="256"/>
+      <c r="F31" s="299"/>
       <c r="G31" s="190" t="s">
         <v>159</v>
       </c>
@@ -6069,10 +6072,10 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="247" t="s">
+      <c r="A32" s="256" t="s">
         <v>214</v>
       </c>
-      <c r="B32" s="249"/>
+      <c r="B32" s="257"/>
       <c r="C32" s="31"/>
       <c r="E32" s="82">
         <v>1</v>
@@ -6082,7 +6085,7 @@
       </c>
       <c r="G32" s="32"/>
       <c r="H32" s="73"/>
-      <c r="I32" s="245"/>
+      <c r="I32" s="276"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="155" t="s">
@@ -6102,7 +6105,7 @@
         <v>5</v>
       </c>
       <c r="H33" s="32"/>
-      <c r="I33" s="245"/>
+      <c r="I33" s="276"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="156" t="s">
@@ -6117,7 +6120,7 @@
       <c r="F34" s="92"/>
       <c r="G34" s="32"/>
       <c r="H34" s="73"/>
-      <c r="I34" s="245"/>
+      <c r="I34" s="276"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="157" t="s">
@@ -6130,7 +6133,7 @@
       <c r="F35" s="92"/>
       <c r="G35" s="32"/>
       <c r="H35" s="32"/>
-      <c r="I35" s="245"/>
+      <c r="I35" s="276"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="157" t="s">
@@ -6143,7 +6146,7 @@
       <c r="F36" s="92"/>
       <c r="G36" s="32"/>
       <c r="H36" s="32"/>
-      <c r="I36" s="245"/>
+      <c r="I36" s="276"/>
     </row>
     <row r="37" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="157" t="s">
@@ -6156,7 +6159,7 @@
       <c r="F37" s="138"/>
       <c r="G37" s="70"/>
       <c r="H37" s="70"/>
-      <c r="I37" s="246"/>
+      <c r="I37" s="277"/>
     </row>
     <row r="38" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="158" t="s">
@@ -6169,17 +6172,17 @@
       <c r="B39" s="119"/>
     </row>
     <row r="40" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="E40" s="247" t="s">
+      <c r="E40" s="256" t="s">
         <v>187</v>
       </c>
-      <c r="F40" s="248"/>
-      <c r="G40" s="248"/>
-      <c r="H40" s="248"/>
-      <c r="I40" s="249"/>
+      <c r="F40" s="278"/>
+      <c r="G40" s="278"/>
+      <c r="H40" s="278"/>
+      <c r="I40" s="257"/>
     </row>
     <row r="41" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="E41" s="253"/>
-      <c r="F41" s="254"/>
+      <c r="E41" s="296"/>
+      <c r="F41" s="297"/>
       <c r="G41" s="81" t="s">
         <v>159</v>
       </c>
@@ -6197,7 +6200,7 @@
       <c r="F42" s="92"/>
       <c r="G42" s="32"/>
       <c r="H42" s="73"/>
-      <c r="I42" s="245"/>
+      <c r="I42" s="276"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E43" s="82">
@@ -6206,7 +6209,7 @@
       <c r="F43" s="92"/>
       <c r="G43" s="32"/>
       <c r="H43" s="32"/>
-      <c r="I43" s="245"/>
+      <c r="I43" s="276"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E44" s="82">
@@ -6215,7 +6218,7 @@
       <c r="F44" s="92"/>
       <c r="G44" s="32"/>
       <c r="H44" s="73"/>
-      <c r="I44" s="245"/>
+      <c r="I44" s="276"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E45" s="82">
@@ -6224,7 +6227,7 @@
       <c r="F45" s="92"/>
       <c r="G45" s="32"/>
       <c r="H45" s="32"/>
-      <c r="I45" s="245"/>
+      <c r="I45" s="276"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E46" s="82">
@@ -6233,7 +6236,7 @@
       <c r="F46" s="92"/>
       <c r="G46" s="32"/>
       <c r="H46" s="32"/>
-      <c r="I46" s="245"/>
+      <c r="I46" s="276"/>
     </row>
     <row r="47" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E47" s="83">
@@ -6242,11 +6245,25 @@
       <c r="F47" s="138"/>
       <c r="G47" s="70"/>
       <c r="H47" s="70"/>
-      <c r="I47" s="246"/>
+      <c r="I47" s="277"/>
     </row>
     <row r="48" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="I42:I47"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I25:I27"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A8:K8"/>
+    <mergeCell ref="A9:K9"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A16:B16"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A3:B3"/>
@@ -6262,20 +6279,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="I32:I37"/>
     <mergeCell ref="E30:I30"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A8:K8"/>
-    <mergeCell ref="A9:K9"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="I42:I47"/>
-    <mergeCell ref="E40:I40"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I25:I27"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6289,7 +6292,7 @@
   </sheetPr>
   <dimension ref="A1:R68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -6315,32 +6318,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="293" t="s">
+      <c r="A1" s="304" t="s">
         <v>352</v>
       </c>
-      <c r="B1" s="294"/>
-      <c r="C1" s="294"/>
-      <c r="D1" s="294"/>
-      <c r="E1" s="294"/>
-      <c r="F1" s="294"/>
-      <c r="G1" s="294"/>
-      <c r="H1" s="294"/>
-      <c r="I1" s="294"/>
-      <c r="J1" s="295"/>
+      <c r="B1" s="305"/>
+      <c r="C1" s="305"/>
+      <c r="D1" s="305"/>
+      <c r="E1" s="305"/>
+      <c r="F1" s="305"/>
+      <c r="G1" s="305"/>
+      <c r="H1" s="305"/>
+      <c r="I1" s="305"/>
+      <c r="J1" s="306"/>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="296" t="s">
+      <c r="A2" s="307" t="s">
         <v>215</v>
       </c>
-      <c r="B2" s="297"/>
-      <c r="C2" s="297"/>
-      <c r="D2" s="297"/>
-      <c r="E2" s="297"/>
-      <c r="F2" s="297"/>
-      <c r="G2" s="297"/>
-      <c r="H2" s="297"/>
-      <c r="I2" s="297"/>
-      <c r="J2" s="298"/>
+      <c r="B2" s="308"/>
+      <c r="C2" s="308"/>
+      <c r="D2" s="308"/>
+      <c r="E2" s="308"/>
+      <c r="F2" s="308"/>
+      <c r="G2" s="308"/>
+      <c r="H2" s="308"/>
+      <c r="I2" s="308"/>
+      <c r="J2" s="309"/>
       <c r="K2" s="78"/>
       <c r="L2" s="78"/>
       <c r="M2" s="74"/>
@@ -6354,13 +6357,13 @@
       <c r="B3" s="169" t="s">
         <v>290</v>
       </c>
-      <c r="C3" s="299" t="s">
+      <c r="C3" s="310" t="s">
         <v>263</v>
       </c>
-      <c r="D3" s="300"/>
-      <c r="E3" s="300"/>
-      <c r="F3" s="300"/>
-      <c r="G3" s="301"/>
+      <c r="D3" s="311"/>
+      <c r="E3" s="311"/>
+      <c r="F3" s="311"/>
+      <c r="G3" s="312"/>
       <c r="H3" s="169" t="s">
         <v>291</v>
       </c>
@@ -6938,26 +6941,26 @@
       <c r="K23" s="191"/>
     </row>
     <row r="24" spans="1:18" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="385" t="s">
+      <c r="A24" s="325" t="s">
         <v>216</v>
       </c>
-      <c r="B24" s="386"/>
-      <c r="C24" s="386"/>
-      <c r="D24" s="386"/>
-      <c r="E24" s="386"/>
-      <c r="F24" s="386"/>
-      <c r="G24" s="386"/>
-      <c r="H24" s="386"/>
-      <c r="I24" s="386"/>
-      <c r="J24" s="386"/>
-      <c r="K24" s="386"/>
-      <c r="L24" s="386"/>
-      <c r="M24" s="386"/>
-      <c r="N24" s="386"/>
-      <c r="O24" s="386"/>
-      <c r="P24" s="386"/>
-      <c r="Q24" s="386"/>
-      <c r="R24" s="386"/>
+      <c r="B24" s="326"/>
+      <c r="C24" s="326"/>
+      <c r="D24" s="326"/>
+      <c r="E24" s="326"/>
+      <c r="F24" s="326"/>
+      <c r="G24" s="326"/>
+      <c r="H24" s="326"/>
+      <c r="I24" s="326"/>
+      <c r="J24" s="326"/>
+      <c r="K24" s="326"/>
+      <c r="L24" s="326"/>
+      <c r="M24" s="326"/>
+      <c r="N24" s="326"/>
+      <c r="O24" s="326"/>
+      <c r="P24" s="326"/>
+      <c r="Q24" s="326"/>
+      <c r="R24" s="326"/>
     </row>
     <row r="25" spans="1:18" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="135" t="s">
@@ -6996,7 +6999,7 @@
       <c r="L25" s="121" t="s">
         <v>243</v>
       </c>
-      <c r="M25" s="383" t="s">
+      <c r="M25" s="254" t="s">
         <v>243</v>
       </c>
       <c r="N25" s="121" t="s">
@@ -7050,7 +7053,7 @@
       <c r="L26" s="95" t="s">
         <v>94</v>
       </c>
-      <c r="M26" s="384" t="s">
+      <c r="M26" s="255" t="s">
         <v>532</v>
       </c>
       <c r="N26" s="95" t="s">
@@ -7109,70 +7112,70 @@
     </row>
     <row r="28" spans="1:18" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="1:18" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="311" t="s">
+      <c r="A29" s="322" t="s">
         <v>253</v>
       </c>
-      <c r="B29" s="312"/>
-      <c r="C29" s="312"/>
-      <c r="D29" s="312"/>
-      <c r="E29" s="312"/>
-      <c r="F29" s="312"/>
-      <c r="G29" s="312"/>
-      <c r="H29" s="313"/>
+      <c r="B29" s="323"/>
+      <c r="C29" s="323"/>
+      <c r="D29" s="323"/>
+      <c r="E29" s="323"/>
+      <c r="F29" s="323"/>
+      <c r="G29" s="323"/>
+      <c r="H29" s="324"/>
     </row>
     <row r="30" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="302" t="s">
+      <c r="A30" s="313" t="s">
         <v>334</v>
       </c>
-      <c r="B30" s="303"/>
-      <c r="C30" s="303"/>
-      <c r="D30" s="303"/>
-      <c r="E30" s="303"/>
-      <c r="F30" s="303"/>
-      <c r="G30" s="303"/>
-      <c r="H30" s="304"/>
+      <c r="B30" s="314"/>
+      <c r="C30" s="314"/>
+      <c r="D30" s="314"/>
+      <c r="E30" s="314"/>
+      <c r="F30" s="314"/>
+      <c r="G30" s="314"/>
+      <c r="H30" s="315"/>
     </row>
     <row r="31" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="305"/>
-      <c r="B31" s="306"/>
-      <c r="C31" s="306"/>
-      <c r="D31" s="306"/>
-      <c r="E31" s="306"/>
-      <c r="F31" s="306"/>
-      <c r="G31" s="306"/>
-      <c r="H31" s="307"/>
+      <c r="A31" s="316"/>
+      <c r="B31" s="317"/>
+      <c r="C31" s="317"/>
+      <c r="D31" s="317"/>
+      <c r="E31" s="317"/>
+      <c r="F31" s="317"/>
+      <c r="G31" s="317"/>
+      <c r="H31" s="318"/>
     </row>
     <row r="32" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="305"/>
-      <c r="B32" s="306"/>
-      <c r="C32" s="306"/>
-      <c r="D32" s="306"/>
-      <c r="E32" s="306"/>
-      <c r="F32" s="306"/>
-      <c r="G32" s="306"/>
-      <c r="H32" s="307"/>
+      <c r="A32" s="316"/>
+      <c r="B32" s="317"/>
+      <c r="C32" s="317"/>
+      <c r="D32" s="317"/>
+      <c r="E32" s="317"/>
+      <c r="F32" s="317"/>
+      <c r="G32" s="317"/>
+      <c r="H32" s="318"/>
     </row>
     <row r="33" spans="1:10" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="308"/>
-      <c r="B33" s="309"/>
-      <c r="C33" s="309"/>
-      <c r="D33" s="309"/>
-      <c r="E33" s="309"/>
-      <c r="F33" s="309"/>
-      <c r="G33" s="309"/>
-      <c r="H33" s="310"/>
+      <c r="A33" s="319"/>
+      <c r="B33" s="320"/>
+      <c r="C33" s="320"/>
+      <c r="D33" s="320"/>
+      <c r="E33" s="320"/>
+      <c r="F33" s="320"/>
+      <c r="G33" s="320"/>
+      <c r="H33" s="321"/>
     </row>
     <row r="34" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="35" spans="1:10" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A35" s="290" t="s">
+      <c r="A35" s="301" t="s">
         <v>280</v>
       </c>
-      <c r="B35" s="291"/>
-      <c r="C35" s="291"/>
-      <c r="D35" s="291"/>
-      <c r="E35" s="291"/>
-      <c r="F35" s="291"/>
-      <c r="G35" s="292"/>
+      <c r="B35" s="302"/>
+      <c r="C35" s="302"/>
+      <c r="D35" s="302"/>
+      <c r="E35" s="302"/>
+      <c r="F35" s="302"/>
+      <c r="G35" s="303"/>
     </row>
     <row r="36" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="77" t="s">
@@ -7184,12 +7187,12 @@
       <c r="C36" s="77" t="s">
         <v>282</v>
       </c>
-      <c r="D36" s="289" t="s">
+      <c r="D36" s="300" t="s">
         <v>283</v>
       </c>
-      <c r="E36" s="289"/>
-      <c r="F36" s="289"/>
-      <c r="G36" s="289"/>
+      <c r="E36" s="300"/>
+      <c r="F36" s="300"/>
+      <c r="G36" s="300"/>
     </row>
     <row r="37" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -7822,32 +7825,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="111" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="326" t="s">
+      <c r="A1" s="339" t="s">
         <v>353</v>
       </c>
-      <c r="B1" s="327"/>
-      <c r="C1" s="327"/>
-      <c r="D1" s="327"/>
-      <c r="E1" s="327"/>
-      <c r="F1" s="327"/>
-      <c r="G1" s="327"/>
-      <c r="H1" s="327"/>
-      <c r="I1" s="327"/>
-      <c r="J1" s="328"/>
+      <c r="B1" s="340"/>
+      <c r="C1" s="340"/>
+      <c r="D1" s="340"/>
+      <c r="E1" s="340"/>
+      <c r="F1" s="340"/>
+      <c r="G1" s="340"/>
+      <c r="H1" s="340"/>
+      <c r="I1" s="340"/>
+      <c r="J1" s="341"/>
     </row>
     <row r="2" spans="1:10" s="111" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="314" t="s">
+      <c r="A2" s="336" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="315"/>
-      <c r="C2" s="315"/>
-      <c r="D2" s="315"/>
-      <c r="E2" s="315"/>
-      <c r="F2" s="315"/>
-      <c r="G2" s="315"/>
-      <c r="H2" s="315"/>
-      <c r="I2" s="315"/>
-      <c r="J2" s="316"/>
+      <c r="B2" s="337"/>
+      <c r="C2" s="337"/>
+      <c r="D2" s="337"/>
+      <c r="E2" s="337"/>
+      <c r="F2" s="337"/>
+      <c r="G2" s="337"/>
+      <c r="H2" s="337"/>
+      <c r="I2" s="337"/>
+      <c r="J2" s="338"/>
     </row>
     <row r="3" spans="1:10" s="111" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="129" t="s">
@@ -7926,18 +7929,18 @@
       <c r="J5" s="163"/>
     </row>
     <row r="6" spans="1:10" s="111" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="314" t="s">
+      <c r="A6" s="336" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="315"/>
-      <c r="C6" s="315"/>
-      <c r="D6" s="315"/>
-      <c r="E6" s="315"/>
-      <c r="F6" s="315"/>
-      <c r="G6" s="315"/>
-      <c r="H6" s="315"/>
-      <c r="I6" s="315"/>
-      <c r="J6" s="316"/>
+      <c r="B6" s="337"/>
+      <c r="C6" s="337"/>
+      <c r="D6" s="337"/>
+      <c r="E6" s="337"/>
+      <c r="F6" s="337"/>
+      <c r="G6" s="337"/>
+      <c r="H6" s="337"/>
+      <c r="I6" s="337"/>
+      <c r="J6" s="338"/>
     </row>
     <row r="7" spans="1:10" s="111" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="122" t="s">
@@ -7988,18 +7991,18 @@
       <c r="J9" s="71"/>
     </row>
     <row r="10" spans="1:10" s="111" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="314" t="s">
+      <c r="A10" s="336" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="315"/>
-      <c r="C10" s="315"/>
-      <c r="D10" s="315"/>
-      <c r="E10" s="315"/>
-      <c r="F10" s="315"/>
-      <c r="G10" s="315"/>
-      <c r="H10" s="315"/>
-      <c r="I10" s="315"/>
-      <c r="J10" s="316"/>
+      <c r="B10" s="337"/>
+      <c r="C10" s="337"/>
+      <c r="D10" s="337"/>
+      <c r="E10" s="337"/>
+      <c r="F10" s="337"/>
+      <c r="G10" s="337"/>
+      <c r="H10" s="337"/>
+      <c r="I10" s="337"/>
+      <c r="J10" s="338"/>
     </row>
     <row r="11" spans="1:10" s="111" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="125"/>
@@ -8154,18 +8157,18 @@
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10" s="111" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="330" t="s">
+      <c r="A17" s="343" t="s">
         <v>487</v>
       </c>
-      <c r="B17" s="331"/>
-      <c r="C17" s="331"/>
-      <c r="D17" s="331"/>
-      <c r="E17" s="331"/>
-      <c r="F17" s="331"/>
-      <c r="G17" s="331"/>
-      <c r="H17" s="331"/>
-      <c r="I17" s="331"/>
-      <c r="J17" s="332"/>
+      <c r="B17" s="344"/>
+      <c r="C17" s="344"/>
+      <c r="D17" s="344"/>
+      <c r="E17" s="344"/>
+      <c r="F17" s="344"/>
+      <c r="G17" s="344"/>
+      <c r="H17" s="344"/>
+      <c r="I17" s="344"/>
+      <c r="J17" s="345"/>
     </row>
     <row r="18" spans="1:10" s="111" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="215"/>
@@ -8238,18 +8241,18 @@
       <c r="J21" s="229"/>
     </row>
     <row r="22" spans="1:10" s="111" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="314" t="s">
+      <c r="A22" s="336" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="315"/>
-      <c r="C22" s="315"/>
-      <c r="D22" s="315"/>
-      <c r="E22" s="315"/>
-      <c r="F22" s="315"/>
-      <c r="G22" s="315"/>
-      <c r="H22" s="315"/>
-      <c r="I22" s="315"/>
-      <c r="J22" s="316"/>
+      <c r="B22" s="337"/>
+      <c r="C22" s="337"/>
+      <c r="D22" s="337"/>
+      <c r="E22" s="337"/>
+      <c r="F22" s="337"/>
+      <c r="G22" s="337"/>
+      <c r="H22" s="337"/>
+      <c r="I22" s="337"/>
+      <c r="J22" s="338"/>
     </row>
     <row r="23" spans="1:10" s="111" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="129" t="s">
@@ -8312,18 +8315,18 @@
       <c r="J25" s="9"/>
     </row>
     <row r="26" spans="1:10" s="111" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="330" t="s">
+      <c r="A26" s="343" t="s">
         <v>491</v>
       </c>
-      <c r="B26" s="331"/>
-      <c r="C26" s="331"/>
-      <c r="D26" s="331"/>
-      <c r="E26" s="331"/>
-      <c r="F26" s="331"/>
-      <c r="G26" s="331"/>
-      <c r="H26" s="331"/>
-      <c r="I26" s="331"/>
-      <c r="J26" s="332"/>
+      <c r="B26" s="344"/>
+      <c r="C26" s="344"/>
+      <c r="D26" s="344"/>
+      <c r="E26" s="344"/>
+      <c r="F26" s="344"/>
+      <c r="G26" s="344"/>
+      <c r="H26" s="344"/>
+      <c r="I26" s="344"/>
+      <c r="J26" s="345"/>
     </row>
     <row r="27" spans="1:10" s="111" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="230" t="s">
@@ -8390,18 +8393,18 @@
       <c r="J29" s="244"/>
     </row>
     <row r="30" spans="1:10" s="111" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="314" t="s">
+      <c r="A30" s="336" t="s">
         <v>153</v>
       </c>
-      <c r="B30" s="315"/>
-      <c r="C30" s="315"/>
-      <c r="D30" s="315"/>
-      <c r="E30" s="315"/>
-      <c r="F30" s="315"/>
-      <c r="G30" s="315"/>
-      <c r="H30" s="315"/>
-      <c r="I30" s="315"/>
-      <c r="J30" s="316"/>
+      <c r="B30" s="337"/>
+      <c r="C30" s="337"/>
+      <c r="D30" s="337"/>
+      <c r="E30" s="337"/>
+      <c r="F30" s="337"/>
+      <c r="G30" s="337"/>
+      <c r="H30" s="337"/>
+      <c r="I30" s="337"/>
+      <c r="J30" s="338"/>
     </row>
     <row r="31" spans="1:10" s="111" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="129" t="s">
@@ -8463,58 +8466,58 @@
     </row>
     <row r="34" spans="1:10" s="111" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="1:10" s="111" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="317" t="s">
+      <c r="A35" s="327" t="s">
         <v>253</v>
       </c>
-      <c r="B35" s="318"/>
-      <c r="C35" s="318"/>
-      <c r="D35" s="318"/>
-      <c r="E35" s="318"/>
-      <c r="F35" s="318"/>
-      <c r="G35" s="318"/>
-      <c r="H35" s="319"/>
+      <c r="B35" s="328"/>
+      <c r="C35" s="328"/>
+      <c r="D35" s="328"/>
+      <c r="E35" s="328"/>
+      <c r="F35" s="328"/>
+      <c r="G35" s="328"/>
+      <c r="H35" s="329"/>
     </row>
     <row r="36" spans="1:10" s="111" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="320" t="s">
+      <c r="A36" s="330" t="s">
         <v>333</v>
       </c>
-      <c r="B36" s="321"/>
-      <c r="C36" s="321"/>
-      <c r="D36" s="321"/>
-      <c r="E36" s="321"/>
-      <c r="F36" s="321"/>
-      <c r="G36" s="321"/>
-      <c r="H36" s="322"/>
+      <c r="B36" s="331"/>
+      <c r="C36" s="331"/>
+      <c r="D36" s="331"/>
+      <c r="E36" s="331"/>
+      <c r="F36" s="331"/>
+      <c r="G36" s="331"/>
+      <c r="H36" s="332"/>
     </row>
     <row r="37" spans="1:10" s="111" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="320"/>
-      <c r="B37" s="321"/>
-      <c r="C37" s="321"/>
-      <c r="D37" s="321"/>
-      <c r="E37" s="321"/>
-      <c r="F37" s="321"/>
-      <c r="G37" s="321"/>
-      <c r="H37" s="322"/>
+      <c r="A37" s="330"/>
+      <c r="B37" s="331"/>
+      <c r="C37" s="331"/>
+      <c r="D37" s="331"/>
+      <c r="E37" s="331"/>
+      <c r="F37" s="331"/>
+      <c r="G37" s="331"/>
+      <c r="H37" s="332"/>
     </row>
     <row r="38" spans="1:10" s="111" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="320"/>
-      <c r="B38" s="321"/>
-      <c r="C38" s="321"/>
-      <c r="D38" s="321"/>
-      <c r="E38" s="321"/>
-      <c r="F38" s="321"/>
-      <c r="G38" s="321"/>
-      <c r="H38" s="322"/>
+      <c r="A38" s="330"/>
+      <c r="B38" s="331"/>
+      <c r="C38" s="331"/>
+      <c r="D38" s="331"/>
+      <c r="E38" s="331"/>
+      <c r="F38" s="331"/>
+      <c r="G38" s="331"/>
+      <c r="H38" s="332"/>
     </row>
     <row r="39" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="323"/>
-      <c r="B39" s="324"/>
-      <c r="C39" s="324"/>
-      <c r="D39" s="324"/>
-      <c r="E39" s="324"/>
-      <c r="F39" s="324"/>
-      <c r="G39" s="324"/>
-      <c r="H39" s="325"/>
+      <c r="A39" s="333"/>
+      <c r="B39" s="334"/>
+      <c r="C39" s="334"/>
+      <c r="D39" s="334"/>
+      <c r="E39" s="334"/>
+      <c r="F39" s="334"/>
+      <c r="G39" s="334"/>
+      <c r="H39" s="335"/>
       <c r="I39" s="111"/>
       <c r="J39" s="111"/>
     </row>
@@ -8531,15 +8534,15 @@
       <c r="J40" s="111"/>
     </row>
     <row r="41" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A41" s="329" t="s">
+      <c r="A41" s="342" t="s">
         <v>280</v>
       </c>
-      <c r="B41" s="329"/>
-      <c r="C41" s="329"/>
-      <c r="D41" s="329"/>
-      <c r="E41" s="329"/>
-      <c r="F41" s="329"/>
-      <c r="G41" s="329"/>
+      <c r="B41" s="342"/>
+      <c r="C41" s="342"/>
+      <c r="D41" s="342"/>
+      <c r="E41" s="342"/>
+      <c r="F41" s="342"/>
+      <c r="G41" s="342"/>
       <c r="H41" s="111"/>
       <c r="I41" s="111"/>
       <c r="J41" s="111"/>
@@ -8554,12 +8557,12 @@
       <c r="C42" s="77" t="s">
         <v>282</v>
       </c>
-      <c r="D42" s="289" t="s">
+      <c r="D42" s="300" t="s">
         <v>283</v>
       </c>
-      <c r="E42" s="289"/>
-      <c r="F42" s="289"/>
-      <c r="G42" s="289"/>
+      <c r="E42" s="300"/>
+      <c r="F42" s="300"/>
+      <c r="G42" s="300"/>
       <c r="H42" s="111"/>
       <c r="I42" s="111"/>
       <c r="J42" s="111"/>
@@ -8822,14 +8825,14 @@
       <c r="Q1" s="30"/>
     </row>
     <row r="2" spans="1:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="338" t="s">
+      <c r="A2" s="361" t="s">
         <v>252</v>
       </c>
-      <c r="B2" s="339"/>
-      <c r="C2" s="339"/>
-      <c r="D2" s="339"/>
-      <c r="E2" s="339"/>
-      <c r="F2" s="340"/>
+      <c r="B2" s="362"/>
+      <c r="C2" s="362"/>
+      <c r="D2" s="362"/>
+      <c r="E2" s="362"/>
+      <c r="F2" s="363"/>
       <c r="G2" s="351" t="s">
         <v>219</v>
       </c>
@@ -8838,23 +8841,23 @@
       <c r="J2" s="351"/>
       <c r="K2" s="351"/>
       <c r="L2" s="351"/>
-      <c r="M2" s="334" t="s">
+      <c r="M2" s="357" t="s">
         <v>268</v>
       </c>
-      <c r="N2" s="334"/>
-      <c r="O2" s="334"/>
+      <c r="N2" s="357"/>
+      <c r="O2" s="357"/>
       <c r="P2" s="87"/>
       <c r="Q2" s="87"/>
     </row>
     <row r="3" spans="1:17" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="341" t="s">
+      <c r="A3" s="364" t="s">
         <v>476</v>
       </c>
-      <c r="B3" s="342"/>
-      <c r="C3" s="342"/>
-      <c r="D3" s="342"/>
-      <c r="E3" s="342"/>
-      <c r="F3" s="343"/>
+      <c r="B3" s="365"/>
+      <c r="C3" s="365"/>
+      <c r="D3" s="365"/>
+      <c r="E3" s="365"/>
+      <c r="F3" s="366"/>
       <c r="G3" s="353" t="s">
         <v>274</v>
       </c>
@@ -8875,14 +8878,14 @@
       <c r="P3" s="187"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="344" t="s">
+      <c r="A4" s="367" t="s">
         <v>477</v>
       </c>
-      <c r="B4" s="345"/>
-      <c r="C4" s="345"/>
-      <c r="D4" s="345"/>
-      <c r="E4" s="345"/>
-      <c r="F4" s="346"/>
+      <c r="B4" s="368"/>
+      <c r="C4" s="368"/>
+      <c r="D4" s="368"/>
+      <c r="E4" s="368"/>
+      <c r="F4" s="369"/>
       <c r="G4" s="352" t="s">
         <v>220</v>
       </c>
@@ -8939,12 +8942,12 @@
       <c r="D6" s="348"/>
       <c r="E6" s="348"/>
       <c r="F6" s="349"/>
-      <c r="G6" s="333"/>
-      <c r="H6" s="333"/>
-      <c r="I6" s="333"/>
-      <c r="J6" s="333"/>
-      <c r="K6" s="333"/>
-      <c r="L6" s="333"/>
+      <c r="G6" s="346"/>
+      <c r="H6" s="346"/>
+      <c r="I6" s="346"/>
+      <c r="J6" s="346"/>
+      <c r="K6" s="346"/>
+      <c r="L6" s="346"/>
       <c r="M6" s="209"/>
       <c r="N6" s="209"/>
       <c r="O6" s="210"/>
@@ -8956,12 +8959,12 @@
       <c r="D7" s="348"/>
       <c r="E7" s="348"/>
       <c r="F7" s="349"/>
-      <c r="G7" s="333"/>
-      <c r="H7" s="333"/>
-      <c r="I7" s="333"/>
-      <c r="J7" s="333"/>
-      <c r="K7" s="333"/>
-      <c r="L7" s="333"/>
+      <c r="G7" s="346"/>
+      <c r="H7" s="346"/>
+      <c r="I7" s="346"/>
+      <c r="J7" s="346"/>
+      <c r="K7" s="346"/>
+      <c r="L7" s="346"/>
       <c r="M7" s="209"/>
       <c r="N7" s="209"/>
       <c r="O7" s="210"/>
@@ -8973,29 +8976,29 @@
       <c r="D8" s="348"/>
       <c r="E8" s="348"/>
       <c r="F8" s="349"/>
-      <c r="G8" s="333"/>
-      <c r="H8" s="333"/>
-      <c r="I8" s="333"/>
-      <c r="J8" s="333"/>
-      <c r="K8" s="333"/>
-      <c r="L8" s="333"/>
+      <c r="G8" s="346"/>
+      <c r="H8" s="346"/>
+      <c r="I8" s="346"/>
+      <c r="J8" s="346"/>
+      <c r="K8" s="346"/>
+      <c r="L8" s="346"/>
       <c r="M8" s="209"/>
       <c r="N8" s="209"/>
       <c r="O8" s="210"/>
     </row>
     <row r="9" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:17" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="335" t="s">
+      <c r="A10" s="358" t="s">
         <v>327</v>
       </c>
-      <c r="B10" s="336"/>
-      <c r="C10" s="336"/>
-      <c r="D10" s="336"/>
-      <c r="E10" s="336"/>
-      <c r="F10" s="336"/>
-      <c r="G10" s="336"/>
-      <c r="H10" s="336"/>
-      <c r="I10" s="337"/>
+      <c r="B10" s="359"/>
+      <c r="C10" s="359"/>
+      <c r="D10" s="359"/>
+      <c r="E10" s="359"/>
+      <c r="F10" s="359"/>
+      <c r="G10" s="359"/>
+      <c r="H10" s="359"/>
+      <c r="I10" s="360"/>
     </row>
     <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="129" t="s">
@@ -9010,7 +9013,7 @@
       <c r="D11" s="123" t="s">
         <v>243</v>
       </c>
-      <c r="E11" s="381" t="s">
+      <c r="E11" s="252" t="s">
         <v>243</v>
       </c>
       <c r="F11" s="123" t="s">
@@ -9044,7 +9047,7 @@
       <c r="D12" s="145" t="s">
         <v>94</v>
       </c>
-      <c r="E12" s="382" t="s">
+      <c r="E12" s="253" t="s">
         <v>532</v>
       </c>
       <c r="F12" s="145" t="s">
@@ -9090,69 +9093,69 @@
     </row>
     <row r="14" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="317" t="s">
+      <c r="A15" s="327" t="s">
         <v>253</v>
       </c>
-      <c r="B15" s="318"/>
-      <c r="C15" s="318"/>
-      <c r="D15" s="318"/>
-      <c r="E15" s="318"/>
-      <c r="F15" s="318"/>
-      <c r="G15" s="318"/>
-      <c r="H15" s="319"/>
+      <c r="B15" s="328"/>
+      <c r="C15" s="328"/>
+      <c r="D15" s="328"/>
+      <c r="E15" s="328"/>
+      <c r="F15" s="328"/>
+      <c r="G15" s="328"/>
+      <c r="H15" s="329"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="320" t="s">
+      <c r="A16" s="330" t="s">
         <v>335</v>
       </c>
-      <c r="B16" s="321"/>
-      <c r="C16" s="321"/>
-      <c r="D16" s="321"/>
-      <c r="E16" s="321"/>
-      <c r="F16" s="321"/>
-      <c r="G16" s="321"/>
-      <c r="H16" s="322"/>
+      <c r="B16" s="331"/>
+      <c r="C16" s="331"/>
+      <c r="D16" s="331"/>
+      <c r="E16" s="331"/>
+      <c r="F16" s="331"/>
+      <c r="G16" s="331"/>
+      <c r="H16" s="332"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="320"/>
-      <c r="B17" s="321"/>
-      <c r="C17" s="321"/>
-      <c r="D17" s="321"/>
-      <c r="E17" s="321"/>
-      <c r="F17" s="321"/>
-      <c r="G17" s="321"/>
-      <c r="H17" s="322"/>
+      <c r="A17" s="330"/>
+      <c r="B17" s="331"/>
+      <c r="C17" s="331"/>
+      <c r="D17" s="331"/>
+      <c r="E17" s="331"/>
+      <c r="F17" s="331"/>
+      <c r="G17" s="331"/>
+      <c r="H17" s="332"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="320"/>
-      <c r="B18" s="321"/>
-      <c r="C18" s="321"/>
-      <c r="D18" s="321"/>
-      <c r="E18" s="321"/>
-      <c r="F18" s="321"/>
-      <c r="G18" s="321"/>
-      <c r="H18" s="322"/>
+      <c r="A18" s="330"/>
+      <c r="B18" s="331"/>
+      <c r="C18" s="331"/>
+      <c r="D18" s="331"/>
+      <c r="E18" s="331"/>
+      <c r="F18" s="331"/>
+      <c r="G18" s="331"/>
+      <c r="H18" s="332"/>
     </row>
     <row r="19" spans="1:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="323"/>
-      <c r="B19" s="324"/>
-      <c r="C19" s="324"/>
-      <c r="D19" s="324"/>
-      <c r="E19" s="324"/>
-      <c r="F19" s="324"/>
-      <c r="G19" s="324"/>
-      <c r="H19" s="325"/>
+      <c r="A19" s="333"/>
+      <c r="B19" s="334"/>
+      <c r="C19" s="334"/>
+      <c r="D19" s="334"/>
+      <c r="E19" s="334"/>
+      <c r="F19" s="334"/>
+      <c r="G19" s="334"/>
+      <c r="H19" s="335"/>
     </row>
     <row r="21" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="329" t="s">
+      <c r="A21" s="342" t="s">
         <v>280</v>
       </c>
-      <c r="B21" s="329"/>
-      <c r="C21" s="329"/>
-      <c r="D21" s="329"/>
-      <c r="E21" s="329"/>
-      <c r="F21" s="329"/>
-      <c r="G21" s="329"/>
+      <c r="B21" s="342"/>
+      <c r="C21" s="342"/>
+      <c r="D21" s="342"/>
+      <c r="E21" s="342"/>
+      <c r="F21" s="342"/>
+      <c r="G21" s="342"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="77" t="s">
@@ -9164,12 +9167,12 @@
       <c r="C22" s="77" t="s">
         <v>282</v>
       </c>
-      <c r="D22" s="289" t="s">
+      <c r="D22" s="300" t="s">
         <v>283</v>
       </c>
-      <c r="E22" s="289"/>
-      <c r="F22" s="289"/>
-      <c r="G22" s="289"/>
+      <c r="E22" s="300"/>
+      <c r="F22" s="300"/>
+      <c r="G22" s="300"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -9607,12 +9610,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="A16:H19"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="J6:L6"/>
@@ -9623,16 +9630,12 @@
     <mergeCell ref="J5:L5"/>
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="A6:F6"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="A16:H19"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9761,12 +9764,12 @@
       <c r="J2" s="351"/>
       <c r="K2" s="351"/>
       <c r="L2" s="351"/>
-      <c r="M2" s="334" t="s">
+      <c r="M2" s="357" t="s">
         <v>267</v>
       </c>
-      <c r="N2" s="334"/>
-      <c r="O2" s="334"/>
-      <c r="P2" s="334"/>
+      <c r="N2" s="357"/>
+      <c r="O2" s="357"/>
+      <c r="P2" s="357"/>
       <c r="Q2" s="87"/>
     </row>
     <row r="3" spans="1:17" ht="57" customHeight="1" x14ac:dyDescent="0.25">
@@ -9801,14 +9804,14 @@
       <c r="Q3" s="186"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="344" t="s">
+      <c r="A4" s="367" t="s">
         <v>477</v>
       </c>
-      <c r="B4" s="345"/>
-      <c r="C4" s="345"/>
-      <c r="D4" s="345"/>
-      <c r="E4" s="345"/>
-      <c r="F4" s="346"/>
+      <c r="B4" s="368"/>
+      <c r="C4" s="368"/>
+      <c r="D4" s="368"/>
+      <c r="E4" s="368"/>
+      <c r="F4" s="369"/>
       <c r="G4" s="352" t="s">
         <v>221</v>
       </c>
@@ -9837,14 +9840,14 @@
       <c r="D5" s="348"/>
       <c r="E5" s="348"/>
       <c r="F5" s="349"/>
-      <c r="G5" s="357" t="s">
+      <c r="G5" s="370" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="357"/>
-      <c r="I5" s="357"/>
-      <c r="J5" s="357"/>
-      <c r="K5" s="357"/>
-      <c r="L5" s="357"/>
+      <c r="H5" s="370"/>
+      <c r="I5" s="370"/>
+      <c r="J5" s="370"/>
+      <c r="K5" s="370"/>
+      <c r="L5" s="370"/>
       <c r="M5" s="209" t="s">
         <v>264</v>
       </c>
@@ -9865,14 +9868,14 @@
       <c r="D6" s="348"/>
       <c r="E6" s="348"/>
       <c r="F6" s="349"/>
-      <c r="G6" s="357" t="s">
+      <c r="G6" s="370" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="357"/>
-      <c r="I6" s="357"/>
-      <c r="J6" s="357"/>
-      <c r="K6" s="357"/>
-      <c r="L6" s="357"/>
+      <c r="H6" s="370"/>
+      <c r="I6" s="370"/>
+      <c r="J6" s="370"/>
+      <c r="K6" s="370"/>
+      <c r="L6" s="370"/>
       <c r="M6" s="209"/>
       <c r="N6" s="209"/>
       <c r="O6" s="209" t="s">
@@ -9889,12 +9892,12 @@
       <c r="D7" s="348"/>
       <c r="E7" s="348"/>
       <c r="F7" s="349"/>
-      <c r="G7" s="357"/>
-      <c r="H7" s="357"/>
-      <c r="I7" s="357"/>
-      <c r="J7" s="357"/>
-      <c r="K7" s="357"/>
-      <c r="L7" s="357"/>
+      <c r="G7" s="370"/>
+      <c r="H7" s="370"/>
+      <c r="I7" s="370"/>
+      <c r="J7" s="370"/>
+      <c r="K7" s="370"/>
+      <c r="L7" s="370"/>
       <c r="M7" s="209"/>
       <c r="N7" s="209"/>
       <c r="O7" s="209"/>
@@ -9907,12 +9910,12 @@
       <c r="D8" s="348"/>
       <c r="E8" s="348"/>
       <c r="F8" s="349"/>
-      <c r="G8" s="357"/>
-      <c r="H8" s="357"/>
-      <c r="I8" s="357"/>
-      <c r="J8" s="357"/>
-      <c r="K8" s="357"/>
-      <c r="L8" s="357"/>
+      <c r="G8" s="370"/>
+      <c r="H8" s="370"/>
+      <c r="I8" s="370"/>
+      <c r="J8" s="370"/>
+      <c r="K8" s="370"/>
+      <c r="L8" s="370"/>
       <c r="M8" s="209"/>
       <c r="N8" s="209"/>
       <c r="O8" s="209"/>
@@ -9920,17 +9923,17 @@
     </row>
     <row r="9" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:17" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="335" t="s">
+      <c r="A10" s="358" t="s">
         <v>326</v>
       </c>
-      <c r="B10" s="336"/>
-      <c r="C10" s="336"/>
-      <c r="D10" s="336"/>
-      <c r="E10" s="336"/>
-      <c r="F10" s="336"/>
-      <c r="G10" s="336"/>
-      <c r="H10" s="336"/>
-      <c r="I10" s="337"/>
+      <c r="B10" s="359"/>
+      <c r="C10" s="359"/>
+      <c r="D10" s="359"/>
+      <c r="E10" s="359"/>
+      <c r="F10" s="359"/>
+      <c r="G10" s="359"/>
+      <c r="H10" s="359"/>
+      <c r="I10" s="360"/>
     </row>
     <row r="11" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="129" t="s">
@@ -9945,7 +9948,7 @@
       <c r="D11" s="123" t="s">
         <v>243</v>
       </c>
-      <c r="E11" s="381" t="s">
+      <c r="E11" s="252" t="s">
         <v>243</v>
       </c>
       <c r="F11" s="123" t="s">
@@ -9975,7 +9978,7 @@
       <c r="D12" s="145" t="s">
         <v>94</v>
       </c>
-      <c r="E12" s="382" t="s">
+      <c r="E12" s="253" t="s">
         <v>532</v>
       </c>
       <c r="F12" s="145" t="s">
@@ -10019,69 +10022,69 @@
     </row>
     <row r="14" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="317" t="s">
+      <c r="A15" s="327" t="s">
         <v>253</v>
       </c>
-      <c r="B15" s="318"/>
-      <c r="C15" s="318"/>
-      <c r="D15" s="318"/>
-      <c r="E15" s="318"/>
-      <c r="F15" s="318"/>
-      <c r="G15" s="318"/>
-      <c r="H15" s="319"/>
+      <c r="B15" s="328"/>
+      <c r="C15" s="328"/>
+      <c r="D15" s="328"/>
+      <c r="E15" s="328"/>
+      <c r="F15" s="328"/>
+      <c r="G15" s="328"/>
+      <c r="H15" s="329"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="320" t="s">
+      <c r="A16" s="330" t="s">
         <v>336</v>
       </c>
-      <c r="B16" s="321"/>
-      <c r="C16" s="321"/>
-      <c r="D16" s="321"/>
-      <c r="E16" s="321"/>
-      <c r="F16" s="321"/>
-      <c r="G16" s="321"/>
-      <c r="H16" s="322"/>
+      <c r="B16" s="331"/>
+      <c r="C16" s="331"/>
+      <c r="D16" s="331"/>
+      <c r="E16" s="331"/>
+      <c r="F16" s="331"/>
+      <c r="G16" s="331"/>
+      <c r="H16" s="332"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="320"/>
-      <c r="B17" s="321"/>
-      <c r="C17" s="321"/>
-      <c r="D17" s="321"/>
-      <c r="E17" s="321"/>
-      <c r="F17" s="321"/>
-      <c r="G17" s="321"/>
-      <c r="H17" s="322"/>
+      <c r="A17" s="330"/>
+      <c r="B17" s="331"/>
+      <c r="C17" s="331"/>
+      <c r="D17" s="331"/>
+      <c r="E17" s="331"/>
+      <c r="F17" s="331"/>
+      <c r="G17" s="331"/>
+      <c r="H17" s="332"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="320"/>
-      <c r="B18" s="321"/>
-      <c r="C18" s="321"/>
-      <c r="D18" s="321"/>
-      <c r="E18" s="321"/>
-      <c r="F18" s="321"/>
-      <c r="G18" s="321"/>
-      <c r="H18" s="322"/>
+      <c r="A18" s="330"/>
+      <c r="B18" s="331"/>
+      <c r="C18" s="331"/>
+      <c r="D18" s="331"/>
+      <c r="E18" s="331"/>
+      <c r="F18" s="331"/>
+      <c r="G18" s="331"/>
+      <c r="H18" s="332"/>
     </row>
     <row r="19" spans="1:8" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="323"/>
-      <c r="B19" s="324"/>
-      <c r="C19" s="324"/>
-      <c r="D19" s="324"/>
-      <c r="E19" s="324"/>
-      <c r="F19" s="324"/>
-      <c r="G19" s="324"/>
-      <c r="H19" s="325"/>
+      <c r="A19" s="333"/>
+      <c r="B19" s="334"/>
+      <c r="C19" s="334"/>
+      <c r="D19" s="334"/>
+      <c r="E19" s="334"/>
+      <c r="F19" s="334"/>
+      <c r="G19" s="334"/>
+      <c r="H19" s="335"/>
     </row>
     <row r="21" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="329" t="s">
+      <c r="A21" s="342" t="s">
         <v>280</v>
       </c>
-      <c r="B21" s="329"/>
-      <c r="C21" s="329"/>
-      <c r="D21" s="329"/>
-      <c r="E21" s="329"/>
-      <c r="F21" s="329"/>
-      <c r="G21" s="329"/>
+      <c r="B21" s="342"/>
+      <c r="C21" s="342"/>
+      <c r="D21" s="342"/>
+      <c r="E21" s="342"/>
+      <c r="F21" s="342"/>
+      <c r="G21" s="342"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="77" t="s">
@@ -10093,12 +10096,12 @@
       <c r="C22" s="77" t="s">
         <v>282</v>
       </c>
-      <c r="D22" s="289" t="s">
+      <c r="D22" s="300" t="s">
         <v>283</v>
       </c>
-      <c r="E22" s="289"/>
-      <c r="F22" s="289"/>
-      <c r="G22" s="289"/>
+      <c r="E22" s="300"/>
+      <c r="F22" s="300"/>
+      <c r="G22" s="300"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -10270,6 +10273,13 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G2:L2"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="G3:L3"/>
     <mergeCell ref="A10:I10"/>
     <mergeCell ref="A21:G21"/>
     <mergeCell ref="D22:G22"/>
@@ -10284,13 +10294,6 @@
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="G5:L5"/>
     <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="G2:L2"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="G3:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10356,8 +10359,8 @@
   </sheetPr>
   <dimension ref="A1:M85"/>
   <sheetViews>
-    <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -10372,12 +10375,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="358" t="s">
+      <c r="A1" s="371" t="s">
         <v>222</v>
       </c>
-      <c r="B1" s="359"/>
-      <c r="C1" s="359"/>
-      <c r="D1" s="360"/>
+      <c r="B1" s="372"/>
+      <c r="C1" s="372"/>
+      <c r="D1" s="373"/>
       <c r="E1" s="65"/>
       <c r="F1" s="65"/>
       <c r="G1" s="65"/>
@@ -10452,7 +10455,7 @@
       <c r="B6" s="16" t="s">
         <v>495</v>
       </c>
-      <c r="C6" s="374"/>
+      <c r="C6" s="245"/>
       <c r="D6" s="23">
         <v>1000000</v>
       </c>
@@ -10464,7 +10467,9 @@
       <c r="B7" s="16" t="s">
         <v>496</v>
       </c>
-      <c r="C7" s="375"/>
+      <c r="C7" s="246" t="s">
+        <v>533</v>
+      </c>
       <c r="D7" s="23">
         <v>0</v>
       </c>
@@ -10476,7 +10481,9 @@
       <c r="B8" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="376"/>
+      <c r="C8" s="247">
+        <v>1</v>
+      </c>
       <c r="D8" s="23">
         <v>0</v>
       </c>
@@ -10488,7 +10495,7 @@
       <c r="B9" s="15" t="s">
         <v>498</v>
       </c>
-      <c r="C9" s="376"/>
+      <c r="C9" s="247"/>
       <c r="D9" s="23">
         <v>0</v>
       </c>
@@ -10500,7 +10507,7 @@
       <c r="B10" s="16" t="s">
         <v>500</v>
       </c>
-      <c r="C10" s="374"/>
+      <c r="C10" s="245"/>
       <c r="D10" s="23"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -10522,7 +10529,7 @@
       <c r="B12" s="16" t="s">
         <v>502</v>
       </c>
-      <c r="C12" s="374"/>
+      <c r="C12" s="245"/>
       <c r="D12" s="23">
         <v>10000</v>
       </c>
@@ -10534,7 +10541,7 @@
       <c r="B13" s="16" t="s">
         <v>504</v>
       </c>
-      <c r="C13" s="374"/>
+      <c r="C13" s="245"/>
       <c r="D13" s="23">
         <v>0.1</v>
       </c>
@@ -10546,7 +10553,7 @@
       <c r="B14" s="16" t="s">
         <v>506</v>
       </c>
-      <c r="C14" s="374"/>
+      <c r="C14" s="245"/>
       <c r="D14" s="23"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -10556,7 +10563,7 @@
       <c r="B15" s="16" t="s">
         <v>508</v>
       </c>
-      <c r="C15" s="374"/>
+      <c r="C15" s="245"/>
       <c r="D15" s="23"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -10566,7 +10573,7 @@
       <c r="B16" s="16" t="s">
         <v>510</v>
       </c>
-      <c r="C16" s="374"/>
+      <c r="C16" s="245"/>
       <c r="D16" s="23">
         <v>10</v>
       </c>
@@ -10578,7 +10585,7 @@
       <c r="B17" s="16" t="s">
         <v>512</v>
       </c>
-      <c r="C17" s="374"/>
+      <c r="C17" s="245"/>
       <c r="D17" s="23"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -10588,7 +10595,7 @@
       <c r="B18" s="16" t="s">
         <v>514</v>
       </c>
-      <c r="C18" s="374"/>
+      <c r="C18" s="245"/>
       <c r="D18" s="23"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -10956,8 +10963,8 @@
       <c r="B52" s="17" t="s">
         <v>516</v>
       </c>
-      <c r="C52" s="377"/>
-      <c r="D52" s="378"/>
+      <c r="C52" s="248"/>
+      <c r="D52" s="249"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
@@ -10966,8 +10973,8 @@
       <c r="B53" s="16" t="s">
         <v>518</v>
       </c>
-      <c r="C53" s="375"/>
-      <c r="D53" s="379">
+      <c r="C53" s="246"/>
+      <c r="D53" s="250">
         <v>0.02</v>
       </c>
     </row>
@@ -10978,8 +10985,8 @@
       <c r="B54" s="16" t="s">
         <v>520</v>
       </c>
-      <c r="C54" s="375"/>
-      <c r="D54" s="379"/>
+      <c r="C54" s="246"/>
+      <c r="D54" s="250"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
@@ -10988,8 +10995,8 @@
       <c r="B55" s="16" t="s">
         <v>522</v>
       </c>
-      <c r="C55" s="375"/>
-      <c r="D55" s="379"/>
+      <c r="C55" s="246"/>
+      <c r="D55" s="250"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
@@ -10998,8 +11005,8 @@
       <c r="B56" s="16" t="s">
         <v>524</v>
       </c>
-      <c r="C56" s="375"/>
-      <c r="D56" s="379"/>
+      <c r="C56" s="246"/>
+      <c r="D56" s="250"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
@@ -11008,7 +11015,7 @@
       <c r="B57" s="16" t="s">
         <v>526</v>
       </c>
-      <c r="C57" s="375"/>
+      <c r="C57" s="246"/>
       <c r="D57" s="24" t="s">
         <v>72</v>
       </c>
@@ -11271,7 +11278,7 @@
       <c r="A82" s="21" t="s">
         <v>528</v>
       </c>
-      <c r="B82" s="380" t="s">
+      <c r="B82" s="251" t="s">
         <v>529</v>
       </c>
       <c r="C82" s="173"/>
@@ -11346,23 +11353,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="364" t="s">
+      <c r="A1" s="377" t="s">
         <v>195</v>
       </c>
-      <c r="B1" s="365"/>
-      <c r="C1" s="365"/>
-      <c r="D1" s="365"/>
-      <c r="E1" s="365"/>
-      <c r="F1" s="365"/>
-      <c r="G1" s="365"/>
-      <c r="H1" s="365"/>
-      <c r="I1" s="365"/>
-      <c r="J1" s="365"/>
-      <c r="K1" s="365"/>
-      <c r="L1" s="365"/>
-      <c r="M1" s="365"/>
-      <c r="N1" s="365"/>
-      <c r="O1" s="365"/>
+      <c r="B1" s="378"/>
+      <c r="C1" s="378"/>
+      <c r="D1" s="378"/>
+      <c r="E1" s="378"/>
+      <c r="F1" s="378"/>
+      <c r="G1" s="378"/>
+      <c r="H1" s="378"/>
+      <c r="I1" s="378"/>
+      <c r="J1" s="378"/>
+      <c r="K1" s="378"/>
+      <c r="L1" s="378"/>
+      <c r="M1" s="378"/>
+      <c r="N1" s="378"/>
+      <c r="O1" s="378"/>
     </row>
     <row r="2" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33"/>
@@ -11380,17 +11387,17 @@
       <c r="M2" s="34"/>
     </row>
     <row r="3" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="361" t="s">
+      <c r="B3" s="374" t="s">
         <v>196</v>
       </c>
-      <c r="C3" s="362"/>
-      <c r="D3" s="362"/>
-      <c r="E3" s="362"/>
-      <c r="F3" s="362"/>
-      <c r="G3" s="362"/>
-      <c r="H3" s="362"/>
-      <c r="I3" s="362"/>
-      <c r="J3" s="363"/>
+      <c r="C3" s="375"/>
+      <c r="D3" s="375"/>
+      <c r="E3" s="375"/>
+      <c r="F3" s="375"/>
+      <c r="G3" s="375"/>
+      <c r="H3" s="375"/>
+      <c r="I3" s="375"/>
+      <c r="J3" s="376"/>
     </row>
     <row r="4" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B4" s="36"/>
@@ -11581,21 +11588,21 @@
     </row>
     <row r="18" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="2:14" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B19" s="361" t="s">
+      <c r="B19" s="374" t="s">
         <v>196</v>
       </c>
-      <c r="C19" s="362"/>
-      <c r="D19" s="362"/>
-      <c r="E19" s="362"/>
-      <c r="F19" s="362"/>
-      <c r="G19" s="362"/>
-      <c r="H19" s="362"/>
-      <c r="I19" s="362"/>
-      <c r="J19" s="362"/>
-      <c r="K19" s="362"/>
-      <c r="L19" s="362"/>
-      <c r="M19" s="362"/>
-      <c r="N19" s="363"/>
+      <c r="C19" s="375"/>
+      <c r="D19" s="375"/>
+      <c r="E19" s="375"/>
+      <c r="F19" s="375"/>
+      <c r="G19" s="375"/>
+      <c r="H19" s="375"/>
+      <c r="I19" s="375"/>
+      <c r="J19" s="375"/>
+      <c r="K19" s="375"/>
+      <c r="L19" s="375"/>
+      <c r="M19" s="375"/>
+      <c r="N19" s="376"/>
     </row>
     <row r="20" spans="2:14" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B20" s="36"/>
@@ -11797,27 +11804,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="369" t="s">
+      <c r="A1" s="382" t="s">
         <v>206</v>
       </c>
-      <c r="B1" s="370"/>
-      <c r="C1" s="370"/>
-      <c r="D1" s="370"/>
-      <c r="E1" s="370"/>
-      <c r="F1" s="370"/>
-      <c r="G1" s="370"/>
-      <c r="H1" s="370"/>
-      <c r="I1" s="370"/>
-      <c r="J1" s="370"/>
-      <c r="K1" s="370"/>
-      <c r="L1" s="370"/>
-      <c r="M1" s="370"/>
-      <c r="N1" s="370"/>
-      <c r="O1" s="370"/>
-      <c r="P1" s="370"/>
-      <c r="Q1" s="370"/>
-      <c r="R1" s="370"/>
-      <c r="S1" s="370"/>
+      <c r="B1" s="383"/>
+      <c r="C1" s="383"/>
+      <c r="D1" s="383"/>
+      <c r="E1" s="383"/>
+      <c r="F1" s="383"/>
+      <c r="G1" s="383"/>
+      <c r="H1" s="383"/>
+      <c r="I1" s="383"/>
+      <c r="J1" s="383"/>
+      <c r="K1" s="383"/>
+      <c r="L1" s="383"/>
+      <c r="M1" s="383"/>
+      <c r="N1" s="383"/>
+      <c r="O1" s="383"/>
+      <c r="P1" s="383"/>
+      <c r="Q1" s="383"/>
+      <c r="R1" s="383"/>
+      <c r="S1" s="383"/>
     </row>
     <row r="2" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="34"/>
@@ -11831,26 +11838,26 @@
       <c r="I2" s="34"/>
     </row>
     <row r="3" spans="1:20" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="361" t="s">
+      <c r="B3" s="374" t="s">
         <v>196</v>
       </c>
-      <c r="C3" s="362"/>
-      <c r="D3" s="362"/>
-      <c r="E3" s="362"/>
-      <c r="F3" s="362"/>
-      <c r="G3" s="362"/>
-      <c r="H3" s="362"/>
-      <c r="I3" s="362"/>
-      <c r="J3" s="363"/>
-      <c r="L3" s="366" t="s">
+      <c r="C3" s="375"/>
+      <c r="D3" s="375"/>
+      <c r="E3" s="375"/>
+      <c r="F3" s="375"/>
+      <c r="G3" s="375"/>
+      <c r="H3" s="375"/>
+      <c r="I3" s="375"/>
+      <c r="J3" s="376"/>
+      <c r="L3" s="379" t="s">
         <v>196</v>
       </c>
-      <c r="M3" s="367"/>
-      <c r="N3" s="367"/>
-      <c r="O3" s="367"/>
-      <c r="P3" s="367"/>
-      <c r="Q3" s="367"/>
-      <c r="R3" s="368"/>
+      <c r="M3" s="380"/>
+      <c r="N3" s="380"/>
+      <c r="O3" s="380"/>
+      <c r="P3" s="380"/>
+      <c r="Q3" s="380"/>
+      <c r="R3" s="381"/>
       <c r="S3" s="35"/>
       <c r="T3" s="35"/>
     </row>
@@ -12081,23 +12088,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="371" t="s">
+      <c r="A1" s="384" t="s">
         <v>205</v>
       </c>
-      <c r="B1" s="372"/>
-      <c r="C1" s="372"/>
-      <c r="D1" s="372"/>
-      <c r="E1" s="372"/>
-      <c r="F1" s="372"/>
-      <c r="G1" s="372"/>
-      <c r="H1" s="372"/>
-      <c r="I1" s="372"/>
-      <c r="J1" s="372"/>
-      <c r="K1" s="372"/>
-      <c r="L1" s="372"/>
-      <c r="M1" s="372"/>
-      <c r="N1" s="372"/>
-      <c r="O1" s="373"/>
+      <c r="B1" s="385"/>
+      <c r="C1" s="385"/>
+      <c r="D1" s="385"/>
+      <c r="E1" s="385"/>
+      <c r="F1" s="385"/>
+      <c r="G1" s="385"/>
+      <c r="H1" s="385"/>
+      <c r="I1" s="385"/>
+      <c r="J1" s="385"/>
+      <c r="K1" s="385"/>
+      <c r="L1" s="385"/>
+      <c r="M1" s="385"/>
+      <c r="N1" s="385"/>
+      <c r="O1" s="386"/>
     </row>
     <row r="2" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33"/>
@@ -12110,22 +12117,22 @@
       <c r="H2" s="51"/>
     </row>
     <row r="3" spans="1:16" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="361" t="s">
+      <c r="B3" s="374" t="s">
         <v>196</v>
       </c>
-      <c r="C3" s="362"/>
-      <c r="D3" s="362"/>
-      <c r="E3" s="362"/>
-      <c r="F3" s="362"/>
-      <c r="G3" s="362"/>
-      <c r="H3" s="363"/>
-      <c r="J3" s="366" t="s">
+      <c r="C3" s="375"/>
+      <c r="D3" s="375"/>
+      <c r="E3" s="375"/>
+      <c r="F3" s="375"/>
+      <c r="G3" s="375"/>
+      <c r="H3" s="376"/>
+      <c r="J3" s="379" t="s">
         <v>196</v>
       </c>
-      <c r="K3" s="367"/>
-      <c r="L3" s="367"/>
-      <c r="M3" s="367"/>
-      <c r="N3" s="368"/>
+      <c r="K3" s="380"/>
+      <c r="L3" s="380"/>
+      <c r="M3" s="380"/>
+      <c r="N3" s="381"/>
       <c r="O3" s="35"/>
       <c r="P3" s="35"/>
     </row>

</xml_diff>